<commit_message>
Adding guide describing which vars are in which sequences
</commit_message>
<xml_diff>
--- a/acs/sequence_guide.xlsx
+++ b/acs/sequence_guide.xlsx
@@ -481,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>